<commit_message>
Final word lists into stimuli folder, old lists out
</commit_message>
<xml_diff>
--- a/EXPINT/experiment_stimuli/wordlist_pretty_2.xlsx
+++ b/EXPINT/experiment_stimuli/wordlist_pretty_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\git\sourcemem\EXPINT\experiment_stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039DEB98-028F-4F47-A9EE-8B2D79BDA4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AC524B-CAF5-4315-B16F-A0D7F8FBDF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{3B494285-4524-4DD0-B9A9-80ED195AEC89}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="138" xr2:uid="{3B494285-4524-4DD0-B9A9-80ED195AEC89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="450">
   <si>
     <t>Semantic</t>
   </si>
@@ -1407,7 +1407,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1426,6 +1426,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1439,17 +1445,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1910,111 +1987,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA44D123-EE85-4C8A-90C8-799983F2C698}">
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:AL36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21:O36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>6</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>7</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>8</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>9</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>10</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>11</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>12</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>13</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>14</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>15</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="1">
         <v>16</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="1">
         <v>17</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="1">
         <v>18</v>
       </c>
+      <c r="U2" t="s">
+        <v>222</v>
+      </c>
+      <c r="V2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>256</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>356</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>368</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>373</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>407</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>435</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>206</v>
       </c>
       <c r="G3" t="s">
@@ -2045,23 +2176,23 @@
         <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>207</v>
       </c>
       <c r="G4" t="s">
@@ -2092,23 +2223,23 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>208</v>
       </c>
       <c r="G5" t="s">
@@ -2139,23 +2270,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>209</v>
       </c>
       <c r="G6" t="s">
@@ -2186,23 +2317,23 @@
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>210</v>
       </c>
       <c r="G7" t="s">
@@ -2233,23 +2364,23 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>211</v>
       </c>
       <c r="G8" t="s">
@@ -2280,23 +2411,23 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>212</v>
       </c>
       <c r="G9" t="s">
@@ -2327,23 +2458,23 @@
         <v>304</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>213</v>
       </c>
       <c r="G10" t="s">
@@ -2374,23 +2505,23 @@
         <v>305</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>214</v>
       </c>
       <c r="G11" t="s">
@@ -2421,23 +2552,23 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="3" t="s">
         <v>215</v>
       </c>
       <c r="G12" t="s">
@@ -2468,23 +2599,23 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
         <v>216</v>
       </c>
       <c r="G13" t="s">
@@ -2515,23 +2646,23 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>217</v>
       </c>
       <c r="G14" t="s">
@@ -2562,23 +2693,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
         <v>218</v>
       </c>
       <c r="G15" t="s">
@@ -2609,23 +2740,23 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
         <v>219</v>
       </c>
       <c r="G16" t="s">
@@ -2660,19 +2791,19 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>220</v>
       </c>
       <c r="G17" t="s">
@@ -2707,19 +2838,19 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="3" t="s">
         <v>221</v>
       </c>
       <c r="G18" t="s">
@@ -2751,98 +2882,98 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>2</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>3</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>4</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>5</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>6</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>7</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>8</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <v>9</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>10</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="1">
         <v>11</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="1">
         <v>12</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="1">
         <v>13</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20" s="1">
         <v>14</v>
       </c>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G21" t="s">
@@ -2877,19 +3008,19 @@
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="3" t="s">
         <v>84</v>
       </c>
       <c r="G22" t="s">
@@ -2924,19 +3055,19 @@
       <c r="A23">
         <v>3</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
         <v>90</v>
       </c>
       <c r="G23" t="s">
@@ -2971,19 +3102,19 @@
       <c r="A24">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="3" t="s">
         <v>100</v>
       </c>
       <c r="G24" t="s">
@@ -3018,19 +3149,19 @@
       <c r="A25">
         <v>5</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="3" t="s">
         <v>105</v>
       </c>
       <c r="G25" t="s">
@@ -3065,19 +3196,19 @@
       <c r="A26">
         <v>6</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="3" t="s">
         <v>114</v>
       </c>
       <c r="G26" t="s">
@@ -3112,19 +3243,19 @@
       <c r="A27">
         <v>7</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="3" t="s">
         <v>122</v>
       </c>
       <c r="G27" t="s">
@@ -3159,19 +3290,19 @@
       <c r="A28">
         <v>8</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="3" t="s">
         <v>118</v>
       </c>
       <c r="G28" t="s">
@@ -3206,19 +3337,19 @@
       <c r="A29">
         <v>9</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="3" t="s">
         <v>134</v>
       </c>
       <c r="G29" t="s">
@@ -3253,19 +3384,19 @@
       <c r="A30">
         <v>10</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="3" t="s">
         <v>315</v>
       </c>
       <c r="G30" t="s">
@@ -3300,19 +3431,19 @@
       <c r="A31">
         <v>11</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="3" t="s">
         <v>319</v>
       </c>
       <c r="G31" t="s">
@@ -3347,19 +3478,19 @@
       <c r="A32">
         <v>12</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="3" t="s">
         <v>320</v>
       </c>
       <c r="G32" t="s">
@@ -3394,19 +3525,19 @@
       <c r="A33">
         <v>13</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="3" t="s">
         <v>353</v>
       </c>
       <c r="G33" t="s">
@@ -3441,19 +3572,19 @@
       <c r="A34">
         <v>14</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="3" t="s">
         <v>141</v>
       </c>
       <c r="G34" t="s">
@@ -3488,19 +3619,19 @@
       <c r="A35">
         <v>15</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="3" t="s">
         <v>354</v>
       </c>
       <c r="G35" t="s">
@@ -3535,19 +3666,19 @@
       <c r="A36">
         <v>16</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="3" t="s">
         <v>355</v>
       </c>
       <c r="G36" t="s">
@@ -3584,49 +3715,70 @@
     <mergeCell ref="A19:S19"/>
   </mergeCells>
   <conditionalFormatting sqref="P21:P35">
-    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V21">
-    <cfRule type="duplicateValues" dxfId="13" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V21:V36">
-    <cfRule type="duplicateValues" dxfId="12" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D36">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:F36">
+    <cfRule type="duplicateValues" dxfId="17" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21:G36">
+    <cfRule type="duplicateValues" dxfId="16" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21:H36">
+    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21:I36">
+    <cfRule type="duplicateValues" dxfId="14" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21:J36">
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:K36">
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21:L36">
     <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:G36">
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21:H36">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21:I36">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21:J36">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K36">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L21:L36">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E21:E36">
-    <cfRule type="duplicateValues" dxfId="2" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:B36">
-    <cfRule type="duplicateValues" dxfId="1" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C36">
-    <cfRule type="duplicateValues" dxfId="0" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD2">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF2">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG2">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH2">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH2">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change some words in list
drapes and draped both appeared, have substituted with sleeve. cleat i found a bit weird, and swapped for blouse. both substitutes have a frequency of less than 500 (about 200 i think), so fulfill initial requirements
</commit_message>
<xml_diff>
--- a/EXPINT/experiment_stimuli/wordlist_pretty_2.xlsx
+++ b/EXPINT/experiment_stimuli/wordlist_pretty_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\git\sourcemem\EXPINT\experiment_stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AC524B-CAF5-4315-B16F-A0D7F8FBDF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21655ED6-BE00-47AF-B3F5-9B1AB840D08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="138" xr2:uid="{3B494285-4524-4DD0-B9A9-80ED195AEC89}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="450">
   <si>
     <t>Semantic</t>
   </si>
@@ -523,9 +523,6 @@
     <t>skirts</t>
   </si>
   <si>
-    <t>drapes</t>
-  </si>
-  <si>
     <t>tights</t>
   </si>
   <si>
@@ -550,9 +547,6 @@
     <t>cloths</t>
   </si>
   <si>
-    <t>cleats</t>
-  </si>
-  <si>
     <t>garter</t>
   </si>
   <si>
@@ -1385,6 +1379,12 @@
   </si>
   <si>
     <t>debtor</t>
+  </si>
+  <si>
+    <t>sleeve</t>
+  </si>
+  <si>
+    <t>blouse</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1407,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1426,12 +1426,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1445,13 +1439,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1987,15 +1982,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA44D123-EE85-4C8A-90C8-799983F2C698}">
-  <dimension ref="A1:AL36"/>
+  <dimension ref="A1:AM36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2013,12 +2008,32 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1</v>
@@ -2062,74 +2077,32 @@
       <c r="O2" s="1">
         <v>14</v>
       </c>
-      <c r="P2" s="1">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>16</v>
-      </c>
-      <c r="R2" s="1">
-        <v>17</v>
-      </c>
-      <c r="S2" s="1">
-        <v>18</v>
-      </c>
-      <c r="U2" t="s">
-        <v>222</v>
-      </c>
-      <c r="V2" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" t="s">
-        <v>67</v>
-      </c>
-      <c r="X2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>256</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>271</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>299</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>356</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>368</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>373</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>396</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>407</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>435</v>
-      </c>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2137,19 +2110,19 @@
         <v>160</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -2161,22 +2134,46 @@
         <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L3" t="s">
         <v>8</v>
       </c>
       <c r="M3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N3" t="s">
         <v>86</v>
       </c>
       <c r="O3" t="s">
-        <v>299</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2187,13 +2184,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -2205,7 +2202,7 @@
         <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K4" t="s">
         <v>68</v>
@@ -2217,13 +2214,37 @@
         <v>65</v>
       </c>
       <c r="N4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="O4" t="s">
-        <v>300</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2231,28 +2252,28 @@
         <v>161</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K5" t="s">
         <v>49</v>
@@ -2261,21 +2282,45 @@
         <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="N5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="O5" t="s">
         <v>6</v>
       </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>448</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
@@ -2287,104 +2332,152 @@
         <v>7</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I6" t="s">
         <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K6" t="s">
         <v>66</v>
       </c>
       <c r="L6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O6" t="s">
-        <v>301</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L7" t="s">
         <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="N7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O7" t="s">
-        <v>302</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H8" t="s">
         <v>17</v>
@@ -2399,27 +2492,51 @@
         <v>16</v>
       </c>
       <c r="L8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="N8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O8" t="s">
-        <v>303</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>20</v>
@@ -2428,16 +2545,16 @@
         <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H9" t="s">
         <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J9" t="s">
         <v>30</v>
@@ -2446,39 +2563,63 @@
         <v>21</v>
       </c>
       <c r="L9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="N9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="O9" t="s">
-        <v>304</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H10" t="s">
         <v>22</v>
@@ -2487,42 +2628,66 @@
         <v>98</v>
       </c>
       <c r="J10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L10" t="s">
         <v>42</v>
       </c>
       <c r="M10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O10" t="s">
-        <v>305</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G11" t="s">
         <v>45</v>
@@ -2531,95 +2696,143 @@
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J11" t="s">
         <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L11" t="s">
         <v>47</v>
       </c>
       <c r="M11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="O11" t="s">
-        <v>306</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="K12" t="s">
         <v>37</v>
       </c>
       <c r="L12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M12" t="s">
         <v>95</v>
       </c>
       <c r="N12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="O12" t="s">
-        <v>307</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -2628,42 +2841,66 @@
         <v>111</v>
       </c>
       <c r="J13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="N13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="O13" t="s">
-        <v>308</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="3"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G14" t="s">
         <v>130</v>
@@ -2672,10 +2909,10 @@
         <v>43</v>
       </c>
       <c r="I14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K14" t="s">
         <v>154</v>
@@ -2684,7 +2921,7 @@
         <v>50</v>
       </c>
       <c r="M14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N14" t="s">
         <v>138</v>
@@ -2692,55 +2929,103 @@
       <c r="O14" t="s">
         <v>2</v>
       </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>171</v>
+        <v>449</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H15" t="s">
         <v>51</v>
       </c>
       <c r="I15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J15" t="s">
         <v>63</v>
       </c>
       <c r="K15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L15" t="s">
         <v>53</v>
       </c>
       <c r="M15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="N15" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O15" t="s">
         <v>74</v>
       </c>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="3"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2748,75 +3033,99 @@
         <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H16" t="s">
         <v>54</v>
       </c>
       <c r="I16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="M16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="N16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="O16" t="s">
-        <v>309</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I17" t="s">
         <v>158</v>
       </c>
       <c r="J17" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K17" t="s">
         <v>57</v>
@@ -2825,36 +3134,60 @@
         <v>60</v>
       </c>
       <c r="M17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="N17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="O17" t="s">
-        <v>310</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H18" t="s">
         <v>61</v>
@@ -2863,25 +3196,49 @@
         <v>147</v>
       </c>
       <c r="J18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O18" t="s">
-        <v>311</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -2899,12 +3256,32 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>1</v>
@@ -2948,16 +3325,32 @@
       <c r="O20" s="1">
         <v>14</v>
       </c>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2965,25 +3358,25 @@
         <v>69</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H21" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I21" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J21" t="s">
         <v>70</v>
@@ -2992,19 +3385,43 @@
         <v>4</v>
       </c>
       <c r="L21" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M21" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="N21" t="s">
         <v>75</v>
       </c>
       <c r="O21" t="s">
-        <v>435</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+      <c r="AG21" s="3"/>
+      <c r="AH21" s="3"/>
+      <c r="AI21" s="3"/>
+      <c r="AJ21" s="3"/>
+      <c r="AK21" s="3"/>
+      <c r="AL21" s="3"/>
+      <c r="AM21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3012,46 +3429,70 @@
         <v>83</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>84</v>
       </c>
       <c r="G22" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H22" t="s">
         <v>91</v>
       </c>
       <c r="I22" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J22" t="s">
         <v>73</v>
       </c>
       <c r="K22" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L22" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="M22" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="N22" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="O22" t="s">
         <v>32</v>
       </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3059,46 +3500,66 @@
         <v>89</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>90</v>
       </c>
       <c r="G23" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H23" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I23" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J23" t="s">
         <v>80</v>
       </c>
       <c r="K23" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L23" t="s">
         <v>71</v>
       </c>
       <c r="M23" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="N23" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="O23" t="s">
-        <v>436</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3106,46 +3567,66 @@
         <v>94</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H24" t="s">
         <v>96</v>
       </c>
       <c r="I24" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J24" t="s">
         <v>85</v>
       </c>
       <c r="K24" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L24" t="s">
         <v>77</v>
       </c>
       <c r="M24" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="N24" t="s">
         <v>81</v>
       </c>
       <c r="O24" t="s">
-        <v>437</v>
-      </c>
+        <v>435</v>
+      </c>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>5</v>
       </c>
@@ -3156,7 +3637,7 @@
         <v>88</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>76</v>
@@ -3165,81 +3646,121 @@
         <v>105</v>
       </c>
       <c r="G25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H25" t="s">
         <v>101</v>
       </c>
       <c r="I25" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J25" t="s">
         <v>92</v>
       </c>
       <c r="K25" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L25" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M25" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="N25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="O25" t="s">
-        <v>438</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>93</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>114</v>
       </c>
       <c r="G26" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H26" t="s">
         <v>106</v>
       </c>
       <c r="I26" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J26" t="s">
         <v>97</v>
       </c>
       <c r="K26" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L26" t="s">
         <v>58</v>
       </c>
       <c r="M26" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="N26" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="O26" t="s">
-        <v>439</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="3"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>7</v>
       </c>
@@ -3247,10 +3768,10 @@
         <v>104</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>87</v>
@@ -3259,13 +3780,13 @@
         <v>122</v>
       </c>
       <c r="G27" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H27" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I27" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J27" t="s">
         <v>102</v>
@@ -3274,19 +3795,39 @@
         <v>107</v>
       </c>
       <c r="L27" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="N27" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="O27" t="s">
-        <v>440</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>8</v>
       </c>
@@ -3294,46 +3835,66 @@
         <v>112</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>118</v>
       </c>
       <c r="G28" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H28" t="s">
         <v>115</v>
       </c>
       <c r="I28" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J28" t="s">
         <v>108</v>
       </c>
       <c r="K28" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L28" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="M28" t="s">
         <v>26</v>
       </c>
       <c r="N28" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="O28" t="s">
-        <v>441</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="3"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>9</v>
       </c>
@@ -3344,43 +3905,63 @@
         <v>120</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>134</v>
       </c>
       <c r="G29" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H29" t="s">
         <v>123</v>
       </c>
       <c r="I29" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J29" t="s">
         <v>116</v>
       </c>
       <c r="K29" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L29" t="s">
         <v>125</v>
       </c>
       <c r="M29" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="N29" t="s">
         <v>153</v>
       </c>
       <c r="O29" t="s">
-        <v>442</v>
-      </c>
+        <v>440</v>
+      </c>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="3"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>10</v>
       </c>
@@ -3388,46 +3969,46 @@
         <v>126</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G30" t="s">
         <v>35</v>
       </c>
       <c r="H30" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I30" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J30" t="s">
         <v>124</v>
       </c>
       <c r="K30" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L30" t="s">
         <v>131</v>
       </c>
       <c r="M30" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="N30" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="O30" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>11</v>
       </c>
@@ -3435,46 +4016,46 @@
         <v>132</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G31" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H31" t="s">
         <v>127</v>
       </c>
       <c r="I31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J31" t="s">
         <v>128</v>
       </c>
       <c r="K31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="M31" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="N31" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="O31" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>12</v>
       </c>
@@ -3482,43 +4063,43 @@
         <v>139</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G32" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H32" t="s">
         <v>135</v>
       </c>
       <c r="I32" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J32" t="s">
         <v>136</v>
       </c>
       <c r="K32" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L32" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="M32" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="N32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="O32" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
@@ -3529,7 +4110,7 @@
         <v>146</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>117</v>
@@ -3538,7 +4119,7 @@
         <v>110</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G33" t="s">
         <v>133</v>
@@ -3547,25 +4128,25 @@
         <v>142</v>
       </c>
       <c r="I33" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J33" t="s">
         <v>144</v>
       </c>
       <c r="K33" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L33" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M33" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="N33" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="O33" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
@@ -3576,7 +4157,7 @@
         <v>150</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>129</v>
@@ -3594,7 +4175,7 @@
         <v>148</v>
       </c>
       <c r="I34" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J34" t="s">
         <v>149</v>
@@ -3603,16 +4184,16 @@
         <v>143</v>
       </c>
       <c r="L34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M34" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="N34" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="O34" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
@@ -3629,16 +4210,16 @@
         <v>145</v>
       </c>
       <c r="E35" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>354</v>
-      </c>
       <c r="G35" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H35" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I35" t="s">
         <v>56</v>
@@ -3647,19 +4228,19 @@
         <v>152</v>
       </c>
       <c r="K35" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L35" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M35" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="N35" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="O35" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
@@ -3670,7 +4251,7 @@
         <v>159</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>156</v>
@@ -3679,40 +4260,40 @@
         <v>52</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G36" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H36" t="s">
         <v>151</v>
       </c>
       <c r="I36" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J36" t="s">
         <v>155</v>
       </c>
       <c r="K36" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L36" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="M36" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="N36" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="O36" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A19:S19"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A19:O19"/>
   </mergeCells>
   <conditionalFormatting sqref="P21:P35">
     <cfRule type="duplicateValues" dxfId="21" priority="24"/>

</xml_diff>